<commit_message>
新增 README.md 新增 seo_search_keyword 加入排名功能
</commit_message>
<xml_diff>
--- a/seo_search_keyword.xlsx
+++ b/seo_search_keyword.xlsx
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/york/Library/CloudStorage/GoogleDrive-coolyork0503@gmail.com/我的雲端硬碟/業安科技/APP/seo_auto_check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851FF70F-9B05-F445-99A5-C615F862CD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFB9859-10CB-6A42-B304-82858A6BC986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KEYWORDS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -422,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:B18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -434,92 +446,164 @@
     <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="1:2">
+      <c r="A1" t="str">
+        <f>"Total: " &amp; COUNTA(B2:B10000)</f>
+        <v>Total: 17</v>
+      </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <f>IF(B2&lt;&gt;"", COUNTA($B$2:B2), "")</f>
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <f>IF(B3&lt;&gt;"", COUNTA($B$2:B3), "")</f>
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <f>IF(B4&lt;&gt;"", COUNTA($B$2:B4), "")</f>
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <f>IF(B5&lt;&gt;"", COUNTA($B$2:B5), "")</f>
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <f>IF(B6&lt;&gt;"", COUNTA($B$2:B6), "")</f>
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <f>IF(B7&lt;&gt;"", COUNTA($B$2:B7), "")</f>
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <f>IF(B8&lt;&gt;"", COUNTA($B$2:B8), "")</f>
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <f>IF(B9&lt;&gt;"", COUNTA($B$2:B9), "")</f>
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <f>IF(B10&lt;&gt;"", COUNTA($B$2:B10), "")</f>
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <f>IF(B11&lt;&gt;"", COUNTA($B$2:B11), "")</f>
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <f>IF(B12&lt;&gt;"", COUNTA($B$2:B12), "")</f>
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <f>IF(B13&lt;&gt;"", COUNTA($B$2:B13), "")</f>
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <f>IF(B14&lt;&gt;"", COUNTA($B$2:B14), "")</f>
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <f>IF(B15&lt;&gt;"", COUNTA($B$2:B15), "")</f>
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <f>IF(B16&lt;&gt;"", COUNTA($B$2:B16), "")</f>
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <f>IF(B17&lt;&gt;"", COUNTA($B$2:B17), "")</f>
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <f>IF(B18&lt;&gt;"", COUNTA($B$2:B18), "")</f>
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>

</xml_diff>